<commit_message>
updated for apache poi
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataExcel.xlsx
+++ b/src/test/resources/TestDataExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENTHIL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENTHIL\Desktop\PROJECTS\ExcelScreenshot\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46767E57-939D-4658-97E2-EB959901ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0A11CF-39A2-4970-AC55-4F90D8866E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EDBB8968-2D3C-4402-8FE9-B7E7FBB97AA9}"/>
   </bookViews>
@@ -34,54 +34,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>Test Data</t>
-  </si>
-  <si>
-    <t>Welcom</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>asdflkasdf'</t>
-  </si>
-  <si>
-    <t>kdjf</t>
-  </si>
-  <si>
-    <t>sadfasdf</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>hqh</t>
-  </si>
-  <si>
-    <t>jh</t>
-  </si>
-  <si>
-    <t>lh</t>
-  </si>
-  <si>
-    <t>lhl</t>
-  </si>
-  <si>
-    <t>jkl</t>
-  </si>
-  <si>
-    <t>jlk</t>
-  </si>
-  <si>
-    <t>jlkj</t>
-  </si>
-  <si>
-    <t>lj</t>
-  </si>
-  <si>
-    <t>ljlj</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+  <si>
+    <t>adf</t>
+  </si>
+  <si>
+    <t>dfgs</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>sfdg</t>
+  </si>
+  <si>
+    <t>asf</t>
+  </si>
+  <si>
+    <t>gsdf</t>
+  </si>
+  <si>
+    <t>gs</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>sdfgsdfgs</t>
+  </si>
+  <si>
+    <t>gsdfgDSFGsdfGSDFG</t>
+  </si>
+  <si>
+    <t>gds</t>
+  </si>
+  <si>
+    <t>dsfg</t>
+  </si>
+  <si>
+    <t>sdfh</t>
+  </si>
+  <si>
+    <t>gsf</t>
+  </si>
+  <si>
+    <t>gh</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>fdhj</t>
+  </si>
+  <si>
+    <t>sdfgDFg</t>
+  </si>
+  <si>
+    <t>sdfgsdfg</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>sfg</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>fds</t>
+  </si>
+  <si>
+    <t>gcj</t>
   </si>
 </sst>
 </file>
@@ -433,74 +469,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6B4B54-1104-4D65-9830-33E7C768F041}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection sqref="A1:AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="U2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Y2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AA2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="V3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="W3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="Y3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z3" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>